<commit_message>
Update: lecture added to Json
</commit_message>
<xml_diff>
--- a/script/2023 Trimester 1 - T4T6 (revamped).xlsx
+++ b/script/2023 Trimester 1 - T4T6 (revamped).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26685" windowHeight="11880" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="12780" windowHeight="11700" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="T4T6" sheetId="1" r:id="rId1"/>
@@ -664,9 +664,9 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-14809]d/m/yyyy;@"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -689,9 +689,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -704,16 +771,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -734,44 +801,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -779,16 +809,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -797,28 +819,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -839,7 +839,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,103 +917,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -965,13 +947,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,25 +989,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1013,7 +1013,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,35 +1027,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1077,26 +1083,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1110,17 +1099,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1129,61 +1114,76 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8"/>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="6"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="9"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
@@ -87885,7 +87885,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="6"/>

</xml_diff>